<commit_message>
Added pools submission to submission template tests
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Sample_submission_v3_13_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Sample_submission_v3_13_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FF4A80-2EA8-4E41-A918-8E32627F1ACE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE62888-B8A0-2747-81CA-73A92B263C86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,7 +435,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3218" uniqueCount="2934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3251" uniqueCount="2941">
   <si>
     <t>SAMPLE SUBMISSION</t>
   </si>
@@ -9286,6 +9286,27 @@
   </si>
   <si>
     <t>Library Size (bp)</t>
+  </si>
+  <si>
+    <t>Library_for_pool_1</t>
+  </si>
+  <si>
+    <t>Library_for_pool_2</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>SubmittedPool</t>
+  </si>
+  <si>
+    <t>ContainerForPool</t>
+  </si>
+  <si>
+    <t>PoolComment</t>
   </si>
 </sst>
 </file>
@@ -9583,7 +9604,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9656,12 +9677,181 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -10414,15 +10604,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG500"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="V1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
@@ -11157,7 +11347,7 @@
       <c r="AC15" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="AD15" s="31"/>
+      <c r="AD15" s="33"/>
       <c r="AE15" s="31" t="s">
         <v>2931</v>
       </c>
@@ -11166,43 +11356,85 @@
       </c>
     </row>
     <row r="16" spans="1:32">
-      <c r="A16" s="13"/>
+      <c r="A16" s="31" t="s">
+        <v>56</v>
+      </c>
       <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="C16" s="13" t="s">
+        <v>2934</v>
+      </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="14"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
+      <c r="J16" s="13" t="s">
+        <v>2913</v>
+      </c>
       <c r="K16" s="13"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
+      <c r="L16" s="15">
+        <v>9606</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>2914</v>
+      </c>
+      <c r="N16" s="32" t="s">
+        <v>2915</v>
+      </c>
+      <c r="O16" s="32" t="s">
+        <v>2916</v>
+      </c>
+      <c r="P16" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q16" s="32" t="s">
+        <v>2914</v>
+      </c>
       <c r="R16" s="14"/>
       <c r="S16" s="14"/>
-      <c r="T16" s="4"/>
+      <c r="T16" s="4">
+        <v>20</v>
+      </c>
       <c r="U16" s="16"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="14"/>
-      <c r="AC16" s="14"/>
-      <c r="AD16" s="14"/>
+      <c r="V16" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="W16" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="X16" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y16" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z16" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA16" s="36" t="s">
+        <v>2936</v>
+      </c>
+      <c r="AB16" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC16" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD16" s="36" t="s">
+        <v>2938</v>
+      </c>
       <c r="AE16" s="13"/>
       <c r="AF16" s="13"/>
     </row>
     <row r="17" spans="1:32">
-      <c r="A17" s="13"/>
+      <c r="A17" s="31" t="s">
+        <v>56</v>
+      </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
+      <c r="C17" s="13" t="s">
+        <v>2935</v>
+      </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -11219,17 +11451,37 @@
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
       <c r="S17" s="14"/>
-      <c r="T17" s="4"/>
+      <c r="T17" s="4">
+        <v>20</v>
+      </c>
       <c r="U17" s="16"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="14"/>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="14"/>
+      <c r="V17" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="W17" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="X17" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y17" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z17" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA17" s="36" t="s">
+        <v>2937</v>
+      </c>
+      <c r="AB17" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC17" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD17" s="36" t="s">
+        <v>2938</v>
+      </c>
       <c r="AE17" s="13"/>
       <c r="AF17" s="13"/>
     </row>
@@ -27661,91 +27913,146 @@
     <mergeCell ref="H6:I6"/>
   </mergeCells>
   <conditionalFormatting sqref="G16:G500">
-    <cfRule type="expression" dxfId="17" priority="15">
+    <cfRule type="expression" dxfId="28" priority="26">
       <formula>AND($D16&lt;&gt;"Tube", $D16&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W16:W500">
-    <cfRule type="expression" dxfId="16" priority="16">
-      <formula>OR($A16="DNA", $A16="rna")</formula>
+  <conditionalFormatting sqref="W18:W500">
+    <cfRule type="expression" dxfId="27" priority="27">
+      <formula>OR($A18="DNA", $A18="rna")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X16:AD500">
-    <cfRule type="expression" dxfId="15" priority="18">
+  <conditionalFormatting sqref="X18:AD500 AA16:AA17 AD16:AD17">
+    <cfRule type="expression" dxfId="26" priority="29">
       <formula>OR($B$3="Yes")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16:U500">
-    <cfRule type="expression" dxfId="14" priority="19">
+    <cfRule type="expression" dxfId="25" priority="30">
       <formula>OR($A16="DNA", $A16="rna")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M16:S500">
-    <cfRule type="expression" dxfId="13" priority="20">
+  <conditionalFormatting sqref="M17:S500 M16 R16:S16">
+    <cfRule type="expression" dxfId="24" priority="31">
       <formula>OR($L16&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G15">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="23" priority="24">
       <formula>AND($D8&lt;&gt;"Tube", $D8&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W8:W15">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>OR($A8="DNA", $A8="rna")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X8">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>AND($B$3="Yes")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X8:AC15">
-    <cfRule type="expression" dxfId="9" priority="10">
+  <conditionalFormatting sqref="X8:AC15 X16:Z17">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>OR($B$3="Yes")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U8:U15">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>OR($A8="DNA", $A8="rna")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:S15">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>OR($L8&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD8">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>OR($B$3="Yes")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD9">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>OR($B$3="Yes")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD10">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>OR($B$3="Yes")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD12">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>OR($B$3="Yes")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD11">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>OR($B$3="Yes")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD13">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>OR($B$3="Yes")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD14">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>OR($B$3="Yes")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>OR($L16&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O16">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>OR($L16&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P16">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>OR($L16&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q16">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>OR($L16&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W16">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>OR($A16="DNA", $A16="rna")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W17">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>OR($A17="DNA", $A17="rna")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD15">
     <cfRule type="expression" dxfId="4" priority="5">
       <formula>OR($B$3="Yes")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD12">
+  <conditionalFormatting sqref="AB16">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>OR($B$3="Yes")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD11">
+  <conditionalFormatting sqref="AB17">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>OR($B$3="Yes")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD13">
+  <conditionalFormatting sqref="AC16">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>OR($B$3="Yes")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD14">
+  <conditionalFormatting sqref="AC17">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>OR($B$3="Yes")</formula>
     </cfRule>
@@ -27755,11 +28062,11 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W16:W500" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W18:W500" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>INDIRECT(#REF!)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC16:AC500" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC18:AC500" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>INDIRECT(SUBSTITUTE(#REF!," ","_"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -27767,7 +28074,7 @@
       <formula1>INDIRECT("_" &amp; SUBSTITUTE((SUBSTITUTE(#REF!,"-"," "))," ","_"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AC15" xr:uid="{F0F26AD0-EA6D-8145-8470-88677A989A2F}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="AC15:AC17" xr:uid="{F0F26AD0-EA6D-8145-8470-88677A989A2F}">
       <formula1>INDIRECT(SUBSTITUTE(AB15," ","_"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -27799,7 +28106,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A16:A500</xm:sqref>
+          <xm:sqref>A18:A500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
@@ -27817,7 +28124,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>P16:P500</xm:sqref>
+          <xm:sqref>P17:P500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
@@ -27835,7 +28142,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>AB16:AB500</xm:sqref>
+          <xm:sqref>AB18:AB500</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
@@ -27859,7 +28166,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>W15:AB15</xm:sqref>
+          <xm:sqref>W15:AB15 W16:Z16 X17:Z17 AB16:AB17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{25B2F825-599D-FA46-AE04-9DF84D8291D4}">
           <x14:formula1>
@@ -27868,7 +28175,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>A15</xm:sqref>
+          <xm:sqref>A15:A17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{46591C44-4DB0-4948-B532-12FA409CD1E7}">
           <x14:formula1>
@@ -27887,7 +28194,7 @@
   <dimension ref="A1:J500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -27956,15 +28263,27 @@
       <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="13" t="s">
+        <v>2938</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>2939</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>2939</v>
+      </c>
       <c r="E4" s="27"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="H4" s="37">
+        <v>44562</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>2940</v>
+      </c>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:10">
@@ -33520,6 +33839,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -33540,8 +33860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC385"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="Z1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Modified the test template
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Sample_submission_v3_13_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Sample_submission_v3_13_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE62888-B8A0-2747-81CA-73A92B263C86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA84D90-E873-6A49-8568-59820F361930}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleSubmission" sheetId="1" r:id="rId1"/>
@@ -215,29 +215,21 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Use the ID# only:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Use the ID# only:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Homo Sapiens #9606 
-Mus Musculus #10090 
-Sars-Cov-2 #2697049
-Ixodes Scapularis #6945
-Canis Lupus Familiaris #9615
-Escherichia Coli #562
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -245,29 +237,332 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Homo Sapiens #9606 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Leishmania donovani #5661
-Borreliella burgdorferi #139
-Influenza A virus #11320 
-Influenza B virus #11520
-Respiratory syncytial virus #12814
-Pedicularis canadensis #1325716
-Passiflora #3684
-Salvelinus fontinalis #8038
-Salvelinus namaycush #8040
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Mus Musculus #10090 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Sars-Cov-2 #2697049</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Ixodes Scapularis #6945</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Canis Lupus Familiaris #9615</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Escherichia Coli #562</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Leishmania donovani #5661</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Borreliella burgdorferi #139</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Influenza A virus #11320 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Influenza B virus #11520</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Respiratory syncytial virus #12814</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Pedicularis canadensis #1325716</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Passiflora #3684</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Salvelinus fontinalis #8038</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Salvelinus namaycush #8040</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t>Phaseolus vulgaris #3885</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Gasterosteus aculeatus #69293</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
+          </rPr>
+          <t>Gasterosteus aculeatus aculeatus #481459</t>
         </r>
       </text>
     </comment>
@@ -370,8 +665,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Instructions:
 </t>
@@ -380,9 +674,8 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Container Name must be </t>
         </r>
@@ -391,9 +684,8 @@
             <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t>unique.</t>
         </r>
@@ -401,9 +693,8 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve"> If container name is not unique, a unique prefix will be added to it. Only use the following characters for Sample name:</t>
         </r>
@@ -412,9 +703,8 @@
             <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve"> a-z, A-Z, 0-9, period (.), dash (-), underscore ( _ )</t>
         </r>
@@ -422,9 +712,8 @@
           <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
+            <family val="34"/>
           </rPr>
           <t>. DON'T USE ANY SPECIAL CHARACTERS!!</t>
         </r>
@@ -435,7 +724,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3251" uniqueCount="2941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3255" uniqueCount="2945">
   <si>
     <t>SAMPLE SUBMISSION</t>
   </si>
@@ -9308,6 +9597,18 @@
   <si>
     <t>PoolComment</t>
   </si>
+  <si>
+    <t>DNA1_Alias</t>
+  </si>
+  <si>
+    <t>RNA1_Alias</t>
+  </si>
+  <si>
+    <t>Blood1_Alias</t>
+  </si>
+  <si>
+    <t>Expectoration1_Alias</t>
+  </si>
 </sst>
 </file>
 
@@ -9316,7 +9617,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]\-0"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -9400,13 +9701,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -9461,6 +9755,43 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="34"/>
     </font>
   </fonts>
   <fills count="14">
@@ -9604,7 +9935,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9643,22 +9974,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -9668,17 +9999,18 @@
     <xf numFmtId="49" fontId="7" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10296,8 +10628,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Taxons" displayName="Taxons" ref="G1:G17" totalsRowShown="0">
-  <autoFilter ref="G1:G17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Taxons" displayName="Taxons" ref="G1:G19" totalsRowShown="0">
+  <autoFilter ref="G1:G19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Taxon"/>
   </tableColumns>
@@ -10604,8 +10936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG500"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15"/>
@@ -10679,10 +11011,10 @@
       <c r="F6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="35"/>
+      <c r="I6" s="38"/>
       <c r="T6" s="5" t="s">
         <v>4</v>
       </c>
@@ -10798,7 +11130,9 @@
       <c r="B8" s="32" t="s">
         <v>2910</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="27" t="s">
+        <v>2941</v>
+      </c>
       <c r="D8" s="31" t="s">
         <v>82</v>
       </c>
@@ -10870,7 +11204,9 @@
       <c r="B9" s="32" t="s">
         <v>2919</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="27" t="s">
+        <v>2942</v>
+      </c>
       <c r="D9" s="31" t="s">
         <v>82</v>
       </c>
@@ -10940,7 +11276,9 @@
       <c r="B10" s="32" t="s">
         <v>2920</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="27" t="s">
+        <v>2943</v>
+      </c>
       <c r="D10" s="31" t="s">
         <v>82</v>
       </c>
@@ -11008,7 +11346,9 @@
       <c r="B11" s="32" t="s">
         <v>2923</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="37" t="s">
+        <v>2944</v>
+      </c>
       <c r="D11" s="31" t="s">
         <v>82</v>
       </c>
@@ -11412,7 +11752,7 @@
       <c r="Z16" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="AA16" s="36" t="s">
+      <c r="AA16" s="35" t="s">
         <v>2936</v>
       </c>
       <c r="AB16" s="32" t="s">
@@ -11421,7 +11761,7 @@
       <c r="AC16" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="AD16" s="36" t="s">
+      <c r="AD16" s="35" t="s">
         <v>2938</v>
       </c>
       <c r="AE16" s="13"/>
@@ -11470,7 +11810,7 @@
       <c r="Z17" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="AA17" s="36" t="s">
+      <c r="AA17" s="35" t="s">
         <v>2937</v>
       </c>
       <c r="AB17" s="32" t="s">
@@ -11479,7 +11819,7 @@
       <c r="AC17" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="AD17" s="36" t="s">
+      <c r="AD17" s="35" t="s">
         <v>2938</v>
       </c>
       <c r="AE17" s="13"/>
@@ -28193,8 +28533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E12C86F-9055-974D-B3CC-6ACA4D367679}">
   <dimension ref="A1:J500"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -28278,7 +28618,7 @@
       <c r="E4" s="27"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="37">
+      <c r="H4" s="36">
         <v>44562</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -33860,8 +34200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC385"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15"/>
@@ -35147,6 +35487,9 @@
       <c r="F18" t="s">
         <v>84</v>
       </c>
+      <c r="G18">
+        <v>69293</v>
+      </c>
       <c r="O18" t="s">
         <v>376</v>
       </c>
@@ -35202,6 +35545,9 @@
       </c>
       <c r="F19" t="s">
         <v>191</v>
+      </c>
+      <c r="G19">
+        <v>481459</v>
       </c>
       <c r="O19" t="s">
         <v>393</v>

</xml_diff>